<commit_message>
Modificato Backlog con nuove US
</commit_message>
<xml_diff>
--- a/doc/modificabili/Backlog.xlsx
+++ b/doc/modificabili/Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanic\Desktop\UNIVERSITA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanic\IdeaProjects\2022t1\doc\modificabili\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C93C599E-0045-429A-B371-E7A41A651F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589D0531-EB34-4621-85E8-E866C6B01DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5556CC1A-55C8-4CB4-A1D1-07BE8FB5C949}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -89,13 +89,19 @@
   </si>
   <si>
     <t>Iniziata a fine sprint 1, programmata sprint 2</t>
+  </si>
+  <si>
+    <t>Io utente voglio poter vedere una serie di "predizioni" per poter gestire meglio le possibili situazioni future</t>
+  </si>
+  <si>
+    <t>Io utente voglio contattare il sito tramite browser per poter accedere alle sue funzionalità</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +127,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -130,7 +142,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -153,11 +165,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -180,11 +205,20 @@
     <xf numFmtId="12" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -235,233 +269,31 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid"/>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -490,6 +322,48 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -519,76 +393,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -603,13 +407,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FA79F1C-5C36-4AB8-9B44-CA849549A8FA}" name="Tabella1" displayName="Tabella1" ref="A1:D12" headerRowDxfId="27" dataDxfId="25" totalsRowDxfId="26">
-  <autoFilter ref="A1:D12" xr:uid="{9FA79F1C-5C36-4AB8-9B44-CA849549A8FA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FA79F1C-5C36-4AB8-9B44-CA849549A8FA}" name="Tabella1" displayName="Tabella1" ref="A1:D14" headerRowDxfId="8" dataDxfId="7" totalsRowDxfId="6">
+  <autoFilter ref="A1:D14" xr:uid="{9FA79F1C-5C36-4AB8-9B44-CA849549A8FA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0761B24E-B40B-44B5-A0F3-90D76D50D9D6}" name="ID" totalsRowFunction="count" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{F9CFB09D-B5D7-44B6-9B1E-ED5244187209}" name="Storia" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{F0C953CD-6E3E-468F-95FC-1AF2FE7DCEC7}" name="Punteggio" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{52A59C4E-A374-4710-B743-2471AFA4AB72}" name="Stato" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{0761B24E-B40B-44B5-A0F3-90D76D50D9D6}" name="ID" totalsRowFunction="count" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{F9CFB09D-B5D7-44B6-9B1E-ED5244187209}" name="Storia" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F0C953CD-6E3E-468F-95FC-1AF2FE7DCEC7}" name="Punteggio" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{52A59C4E-A374-4710-B743-2471AFA4AB72}" name="Stato" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -912,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59FC276-D339-4702-9E00-14ABB06B2E18}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1086,6 +890,32 @@
         <v>40</v>
       </c>
       <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3">
+        <v>80</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="8">
+        <v>13</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1109,6 +939,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F794D397A076E84FBC9EEDBF2A761A88" ma:contentTypeVersion="4" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="1ef51e1d6c21e2a09ca5faf57c46a92d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f52b552e-9b94-4894-b6dd-a894f24a684b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6272935dcea4b53dbe0c14cae9e8a0b4" ns3:_="">
     <xsd:import namespace="f52b552e-9b94-4894-b6dd-a894f24a684b"/>
@@ -1254,15 +1093,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1270,6 +1100,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E99AA6E9-1824-4A2A-8F4B-5368D1541F04}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DF92D2C-0C79-48F4-B890-25FFAF1AA801}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1283,14 +1121,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E99AA6E9-1824-4A2A-8F4B-5368D1541F04}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>